<commit_message>
doc - save final results and figures for the best performing models
</commit_message>
<xml_diff>
--- a/final_project/results/metrics_macro.xlsx
+++ b/final_project/results/metrics_macro.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="29">
   <si>
     <t xml:space="preserve">model</t>
   </si>
@@ -76,6 +76,9 @@
     <t xml:space="preserve">random forest_corr</t>
   </si>
   <si>
+    <t xml:space="preserve">all_corr</t>
+  </si>
+  <si>
     <t xml:space="preserve">authors</t>
   </si>
   <si>
@@ -95,6 +98,9 @@
   </si>
   <si>
     <t xml:space="preserve">{'activation': 'relu', 'hidden_layer_sizes': [128, 64], 'learning_rate': 'adaptive', 'max_iter': 5000, 'solver': 'sgd'}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{'activation': 'relu', 'hidden_layer_sizes': [20], 'learning_rate': 'adaptive', 'max_iter': 5000, 'solver': 'sgd'}</t>
   </si>
   <si>
     <t xml:space="preserve">{'activation': 'relu', 'hidden_layer_sizes': [20], 'learning_rate': 'constant', 'max_iter': 5000, 'solver': 'adam'}</t>
@@ -391,17 +397,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1048576"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="50.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="90.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="18.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.42"/>
@@ -523,19 +529,19 @@
         <v>14</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>123.429318443384</v>
+        <v>136.873793984982</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>6.84016828261159</v>
+        <v>7.05638092001734</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>0.492165622300035</v>
+        <v>0.451442322824882</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>9.51941929893485</v>
+        <v>9.93564557424806</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>0.511472669309067</v>
+        <v>0.468384856771993</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -624,441 +630,518 @@
         <v>18</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>139.979973592673</v>
+        <v>123.429318443384</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>7.24694579931723</v>
+        <v>6.84016828261159</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>0.431266965605833</v>
+        <v>0.492165622300035</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>10.0841257489019</v>
+        <v>9.51941929893485</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>0.447361187582569</v>
+        <v>0.511472669309067</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>9</v>
-      </c>
       <c r="C10" s="0" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>81.3031889456529</v>
+        <v>139.979973592673</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>5.35936682471787</v>
+        <v>7.24694579931723</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>0.60525287143655</v>
+        <v>0.431266965605833</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>8.01306746203909</v>
+        <v>10.0841257489019</v>
       </c>
       <c r="H10" s="0" t="n">
-        <v>0.607406118711081</v>
+        <v>0.447361187582569</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>21</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>78.1342926689553</v>
+        <v>81.3031889456529</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>5.57042843237904</v>
+        <v>5.35936682471787</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>0.618602989880979</v>
+        <v>0.60525287143655</v>
       </c>
       <c r="G11" s="0" t="n">
-        <v>7.89094524270069</v>
+        <v>8.01306746203909</v>
       </c>
       <c r="H11" s="0" t="n">
-        <v>0.623838686207411</v>
+        <v>0.607406118711081</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>78.4149526730382</v>
+        <v>78.1342926689553</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>5.61437480589397</v>
+        <v>5.57042843237904</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>0.62011383850581</v>
+        <v>0.618602989880979</v>
       </c>
       <c r="G12" s="0" t="n">
-        <v>7.89516540178532</v>
+        <v>7.89094524270069</v>
       </c>
       <c r="H12" s="0" t="n">
-        <v>0.625012738085308</v>
+        <v>0.623838686207411</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>84.0584879625577</v>
+        <v>78.4149526730382</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>5.90058585763032</v>
+        <v>5.61437480589397</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>0.601543134372753</v>
+        <v>0.62011383850581</v>
       </c>
       <c r="G13" s="0" t="n">
-        <v>8.12971140281904</v>
+        <v>7.89516540178532</v>
       </c>
       <c r="H13" s="0" t="n">
-        <v>0.606948528980529</v>
+        <v>0.625012738085308</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>22</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>80.575123706367</v>
+        <v>80.857407321346</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>5.70053979876665</v>
+        <v>5.7268683029627</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>0.606092959782884</v>
+        <v>0.614058145740051</v>
       </c>
       <c r="G14" s="0" t="n">
-        <v>8.01231372752469</v>
+        <v>7.99086294545401</v>
       </c>
       <c r="H14" s="0" t="n">
-        <v>0.610907860266208</v>
+        <v>0.619221037458723</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>80.9775213174231</v>
+        <v>80.575123706367</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>5.70921212340882</v>
+        <v>5.70053979876665</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>0.608700573126749</v>
+        <v>0.606092959782884</v>
       </c>
       <c r="G15" s="0" t="n">
-        <v>8.01576520028432</v>
+        <v>8.01231372752469</v>
       </c>
       <c r="H15" s="0" t="n">
-        <v>0.613450314929883</v>
+        <v>0.610907860266208</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>80.4759512703862</v>
+        <v>79.9615162062374</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>5.74730512407592</v>
+        <v>5.69962878896615</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>0.613737098294629</v>
+        <v>0.612320435753989</v>
       </c>
       <c r="G16" s="0" t="n">
-        <v>7.97538864404933</v>
+        <v>7.96852160114825</v>
       </c>
       <c r="H16" s="0" t="n">
-        <v>0.618733403498939</v>
+        <v>0.616898403028324</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>79.9134999770499</v>
+        <v>80.4759512703862</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>5.65861359845766</v>
+        <v>5.74730512407592</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>0.6137527241857</v>
+        <v>0.613737098294629</v>
       </c>
       <c r="G17" s="0" t="n">
-        <v>7.96170769298696</v>
+        <v>7.97538864404933</v>
       </c>
       <c r="H17" s="0" t="n">
-        <v>0.618229597065856</v>
+        <v>0.618733403498939</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>79.2493132684659</v>
+        <v>84.0584879625577</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>5.30246646814824</v>
+        <v>5.90058585763032</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>0.618443423794228</v>
+        <v>0.601543134372753</v>
       </c>
       <c r="G18" s="0" t="n">
-        <v>7.92450618948622</v>
+        <v>8.12971140281904</v>
       </c>
       <c r="H18" s="0" t="n">
-        <v>0.62181993673031</v>
+        <v>0.606948528980529</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>83.0532339173407</v>
+        <v>79.9134999770499</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>5.37730930544781</v>
+        <v>5.65861359845766</v>
       </c>
       <c r="F19" s="0" t="n">
-        <v>0.616310405295683</v>
+        <v>0.6137527241857</v>
       </c>
       <c r="G19" s="0" t="n">
-        <v>8.02426474556003</v>
+        <v>7.96170769298696</v>
       </c>
       <c r="H19" s="0" t="n">
-        <v>0.620480313004877</v>
+        <v>0.618229597065856</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>81.527909088032</v>
+        <v>79.2493132684659</v>
       </c>
       <c r="E20" s="0" t="n">
-        <v>5.32466937449839</v>
+        <v>5.30246646814824</v>
       </c>
       <c r="F20" s="0" t="n">
-        <v>0.619505927878634</v>
+        <v>0.618443423794228</v>
       </c>
       <c r="G20" s="0" t="n">
-        <v>7.97071401498533</v>
+        <v>7.92450618948622</v>
       </c>
       <c r="H20" s="0" t="n">
-        <v>0.623027115792628</v>
+        <v>0.62181993673031</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>82.215822878305</v>
+        <v>83.0532339173407</v>
       </c>
       <c r="E21" s="0" t="n">
-        <v>5.36265804249786</v>
+        <v>5.37730930544781</v>
       </c>
       <c r="F21" s="0" t="n">
-        <v>0.622171492840462</v>
+        <v>0.616310405295683</v>
       </c>
       <c r="G21" s="0" t="n">
-        <v>7.97926927200173</v>
+        <v>8.02426474556003</v>
       </c>
       <c r="H21" s="0" t="n">
-        <v>0.624761648242096</v>
+        <v>0.620480313004877</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>92.6385076861146</v>
+        <v>81.5631873319203</v>
       </c>
       <c r="E22" s="0" t="n">
-        <v>6.13258507669207</v>
+        <v>5.38466607185225</v>
       </c>
       <c r="F22" s="0" t="n">
-        <v>0.560734271513309</v>
+        <v>0.61852873806166</v>
       </c>
       <c r="G22" s="0" t="n">
-        <v>8.55007096172774</v>
+        <v>7.98555799196988</v>
       </c>
       <c r="H22" s="0" t="n">
-        <v>0.570504650038458</v>
+        <v>0.6223449920808</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>82.0062100260137</v>
+        <v>78.0835715702577</v>
       </c>
       <c r="E23" s="0" t="n">
-        <v>5.36977308508505</v>
+        <v>5.23506725788577</v>
       </c>
       <c r="F23" s="0" t="n">
-        <v>0.619685627425278</v>
+        <v>0.635634087223037</v>
       </c>
       <c r="G23" s="0" t="n">
-        <v>7.98781792060921</v>
+        <v>7.80283561667466</v>
       </c>
       <c r="H23" s="0" t="n">
-        <v>0.622545765923102</v>
+        <v>0.639455020801961</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>91.8519165850961</v>
+        <v>92.6385076861146</v>
       </c>
       <c r="E24" s="0" t="n">
-        <v>5.99820768412173</v>
+        <v>6.13258507669207</v>
       </c>
       <c r="F24" s="0" t="n">
-        <v>0.579352525502742</v>
+        <v>0.560734271513309</v>
       </c>
       <c r="G24" s="0" t="n">
-        <v>8.43418736266556</v>
+        <v>8.55007096172774</v>
       </c>
       <c r="H24" s="0" t="n">
-        <v>0.584292939042452</v>
+        <v>0.570504650038458</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>82.0062100260137</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>5.36977308508505</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>0.619685627425278</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>7.98781792060921</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <v>0.622545765923103</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>91.8519165850961</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>5.99820768412173</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>0.579352525502742</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>8.43418736266557</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <v>0.584292939042452</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D25" s="0" t="n">
+      <c r="C27" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>82.215822878305</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>5.36265804249786</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>0.622171492840462</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>7.97926927200173</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <v>0.624761648242096</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="0" t="n">
         <v>85.5774535747547</v>
       </c>
-      <c r="E25" s="0" t="n">
+      <c r="E28" s="0" t="n">
         <v>5.58367637073834</v>
       </c>
-      <c r="F25" s="0" t="n">
+      <c r="F28" s="0" t="n">
         <v>0.590909579370096</v>
       </c>
-      <c r="G25" s="0" t="n">
+      <c r="G28" s="0" t="n">
         <v>8.22410861103194</v>
       </c>
-      <c r="H25" s="0" t="n">
+      <c r="H28" s="0" t="n">
         <v>0.597199347212664</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>